<commit_message>
Added checks for PAS-12881: Store the VIN Stub used in rating when vin used does not match and user selects valid, non 'other' values from the vehicle details section.
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New8VIN_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New8VIN_UT_SS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Desktop\SUITE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Documents\CSAA\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -629,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AA25" sqref="AA25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,10 +1317,10 @@
         <v>61</v>
       </c>
       <c r="AA6" s="3">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="AB6" s="3">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AC6" s="3" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Added checks for PAS-12881: Minor db cleaner updates
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New8VIN_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New8VIN_UT_SS.xlsx
@@ -313,7 +313,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,6 +323,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -339,11 +345,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -629,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AA25" sqref="AA25"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,119 +783,119 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:38" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>2018</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="5">
         <v>53080</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="5">
         <v>8</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="5">
         <v>214</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="S2" s="3">
+      <c r="S2" s="5">
         <v>2</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V2" s="3">
+      <c r="V2" s="5">
         <v>2</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AA2" s="3">
+      <c r="AA2" s="5">
         <v>42</v>
       </c>
-      <c r="AB2" s="3">
+      <c r="AB2" s="5">
         <v>42</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AD2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AE2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AF2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AG2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AH2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="AI2" s="3">
+      <c r="AI2" s="5">
         <v>20010101</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AK2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AL2" s="5" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pas-730: Partial match splitted
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New8VIN_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New8VIN_UT_SS.xlsx
@@ -23,42 +23,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Petrenko, Viktor (C)</author>
-  </authors>
-  <commentList>
-    <comment ref="AA6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Petrenko, Viktor (C):</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-User for MSRP PAS-730</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="63">
   <si>
     <t>VIN</t>
   </si>
@@ -228,24 +194,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>8L V12</t>
-  </si>
-  <si>
-    <t>4WD</t>
-  </si>
-  <si>
-    <t>VOLKSWAGEN</t>
-  </si>
-  <si>
-    <t>RT</t>
-  </si>
-  <si>
-    <t>7MSRP15H&amp;V</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -265,22 +213,13 @@
   </si>
   <si>
     <t>HHHKN3DD&amp;E</t>
-  </si>
-  <si>
-    <t>PASSAT</t>
-  </si>
-  <si>
-    <t>PASSAT S</t>
-  </si>
-  <si>
-    <t>SEDAN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,19 +240,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -639,11 +565,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AL5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -788,19 +714,19 @@
     </row>
     <row r="2" spans="1:38" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C2" s="5">
         <v>2018</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>51</v>
@@ -904,10 +830,10 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C3" s="3">
         <v>2018</v>
@@ -919,7 +845,7 @@
         <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>28</v>
@@ -1020,10 +946,10 @@
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C4" s="3">
         <v>2018</v>
@@ -1035,7 +961,7 @@
         <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>28</v>
@@ -1136,10 +1062,10 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C5" s="3">
         <v>2018</v>
@@ -1151,7 +1077,7 @@
         <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>28</v>
@@ -1211,7 +1137,7 @@
         <v>37</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="AA5" s="3">
         <v>42</v>
@@ -1247,128 +1173,11 @@
         <v>39</v>
       </c>
       <c r="AL5" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2018</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6" s="3">
-        <v>88888</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="O6" s="3">
-        <v>12</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>214</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="S6" s="3">
-        <v>4</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="V6" s="3">
-        <v>2</v>
-      </c>
-      <c r="W6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="X6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA6" s="3">
-        <v>66</v>
-      </c>
-      <c r="AB6" s="3">
-        <v>55</v>
-      </c>
-      <c r="AC6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AD6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AH6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI6" s="3">
-        <v>20000101</v>
-      </c>
-      <c r="AJ6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AL6" s="3" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>